<commit_message>
Addition of new sheet
New sheet includes deleted finding (.png files)
</commit_message>
<xml_diff>
--- a/analysis_findings.xlsx
+++ b/analysis_findings.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GAURAV SRIVASTAVA\MyProjects\my_git_masters\Google Data Analytics\Case Study 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C4092FD-9F67-4C21-92B1-ECF71B8A5827}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06A784EB-DF08-4E36-A55C-79F7D5E7FD11}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="avg_ride_length" sheetId="1" r:id="rId1"/>
-    <sheet name="count of rides" sheetId="3" r:id="rId2"/>
+    <sheet name="count_of_rides" sheetId="3" r:id="rId2"/>
+    <sheet name="data_viz" sheetId="4" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">avg_ride_length!$C$1:$C$15</definedName>
@@ -2363,7 +2364,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-8E96-4639-88D3-700DA1FE1ACE}"/>
+              <c16:uniqueId val="{00000000-3F41-4B8B-94DF-B3A701CABC37}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2438,7 +2439,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-8E96-4639-88D3-700DA1FE1ACE}"/>
+              <c16:uniqueId val="{00000001-3F41-4B8B-94DF-B3A701CABC37}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2645,6 +2646,683 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr lang="en-IN" sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+                <a:effectLst/>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-IN" sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+                <a:effectLst/>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:rPr>
+              <a:t>Count of rides by day_of_week and member_casual</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.2020220599040107"/>
+          <c:y val="2.8481833954228798E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr lang="en-IN" sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:sysClr>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:pivotFmts>
+      <c:pivotFmt>
+        <c:idx val="0"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="1"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="2"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="3"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+    </c:pivotFmts>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>casual</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="7"/>
+              <c:pt idx="0">
+                <c:v>Mon</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>Tue</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>Wed</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v>Thu</c:v>
+              </c:pt>
+              <c:pt idx="4">
+                <c:v>Fri</c:v>
+              </c:pt>
+              <c:pt idx="5">
+                <c:v>Sat</c:v>
+              </c:pt>
+              <c:pt idx="6">
+                <c:v>Sun</c:v>
+              </c:pt>
+            </c:strLit>
+          </c:cat>
+          <c:val>
+            <c:numLit>
+              <c:formatCode>General</c:formatCode>
+              <c:ptCount val="7"/>
+              <c:pt idx="0">
+                <c:v>154868</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>149850</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>163603</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v>170629</c:v>
+              </c:pt>
+              <c:pt idx="4">
+                <c:v>213189</c:v>
+              </c:pt>
+              <c:pt idx="5">
+                <c:v>342539</c:v>
+              </c:pt>
+              <c:pt idx="6">
+                <c:v>277157</c:v>
+              </c:pt>
+            </c:numLit>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-4852-4C2F-9425-2B26C92DE54F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>member</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="7"/>
+              <c:pt idx="0">
+                <c:v>Mon</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>Tue</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>Wed</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v>Thu</c:v>
+              </c:pt>
+              <c:pt idx="4">
+                <c:v>Fri</c:v>
+              </c:pt>
+              <c:pt idx="5">
+                <c:v>Sat</c:v>
+              </c:pt>
+              <c:pt idx="6">
+                <c:v>Sun</c:v>
+              </c:pt>
+            </c:strLit>
+          </c:cat>
+          <c:val>
+            <c:numLit>
+              <c:formatCode>General</c:formatCode>
+              <c:ptCount val="7"/>
+              <c:pt idx="0">
+                <c:v>329259</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>354069</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>369074</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v>361698</c:v>
+              </c:pt>
+              <c:pt idx="4">
+                <c:v>361894</c:v>
+              </c:pt>
+              <c:pt idx="5">
+                <c:v>353224</c:v>
+              </c:pt>
+              <c:pt idx="6">
+                <c:v>301263</c:v>
+              </c:pt>
+            </c:numLit>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-4852-4C2F-9425-2B26C92DE54F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="65374352"/>
+        <c:axId val="65177632"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="65374352"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="65177632"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="65177632"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="65374352"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:extLst/>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -2765,6 +3443,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -3772,6 +4490,509 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -4319,16 +5540,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>485775</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>133349</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>33337</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>2380</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>628650</xdr:colOff>
-      <xdr:row>49</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>592931</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>116681</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4353,29 +5574,72 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>466724</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>123824</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>85724</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>628649</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>95249</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3">
+        <xdr:cNvPr id="2" name="Chart 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{08FD973D-1634-4425-8469-8695CC816C46}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F800E439-5AAD-4201-9876-3D87976366D6}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>95251</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2DA3FF9B-B841-43D2-83F0-79EF79AEC453}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -4960,7 +6224,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB2B72CC-928F-44E1-98A5-A41518AC7D18}">
   <dimension ref="A1:J15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
@@ -5254,4 +6518,19 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD8C68BD-BCF0-43B1-AB84-611FF84D162D}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q16" sqref="Q16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>